<commit_message>
Fix failed output writing. Add Priority runs.
</commit_message>
<xml_diff>
--- a/Queue.xlsx
+++ b/Queue.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9108"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9108" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="To Run" sheetId="1" r:id="rId1"/>
@@ -20,164 +20,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>C:/GitHub/Epik-Ligands/run_parametrization.py</author>
-  </authors>
-  <commentList>
-    <comment ref="E2" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Verdana"/>
-          </rPr>
-          <t>New run:
-PDB code: PO4; Molecule: Phosphate anion_pH_1.0; pH 1.0
-Retrieving PDB structure from RCSB ligand expo: Phosphate anion_pH_1.0-rcsb_download.pdb.
-Parsing PDB file.
-Retrieving SDF structure from RCSB ligand expo: Phosphate anion_pH_1.0-rcsb_download.sdf.
-Parsing SDF file.
-Canonicalizing atom names.
-Assign atom type names.
-Running Epik.
-Epik run completed.
-Assigning charges to protonation states.
-State 1
-Charging completed.
-Writing Epik data for state 1
-Run completed.
-Status: Success</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Verdana"/>
-          </rPr>
-          <t>New run:
-PDB code: PO4; Molecule: Phosphate anion_pH_1.0; pH 1.0
-Retrieving PDB structure from RCSB ligand expo: Phosphate anion_pH_1.0-rcsb_download.pdb.
-Parsing PDB file.
-Retrieving SDF structure from RCSB ligand expo: Phosphate anion_pH_1.0-rcsb_download.sdf.
-Parsing SDF file.
-Canonicalizing atom names.
-Assign atom type names.
-Running Epik.
-Epik run completed.
-Assigning charges to protonation states.
-State 1
-Charging completed.
-Writing Epik data for state 1
-Run completed.
-Status: Success
-New run:
-PDB code: PO4; Molecule: Phosphate anion_pH_3.0; pH 3.0
-Retrieving PDB structure from RCSB ligand expo: Phosphate anion_pH_3.0-rcsb_download.pdb.
-Parsing PDB file.
-Retrieving SDF structure from RCSB ligand expo: Phosphate anion_pH_3.0-rcsb_download.sdf.
-Parsing SDF file.
-Canonicalizing atom names.
-Assign atom type names.
-Running Epik.
-Epik run completed.
-Assigning charges to protonation states.
-State 1
-Charging completed.
-Writing Epik data for state 1
-Run completed.
-Status: Success</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Verdana"/>
-          </rPr>
-          <t>New run:
-PDB code: SO4; Molecule: Sulfate anion_pH_2.0; pH 2.0
-Retrieving PDB structure from RCSB ligand expo: Sulfate anion_pH_2.0-rcsb_download.pdb.
-Parsing PDB file.
-Retrieving SDF structure from RCSB ligand expo: Sulfate anion_pH_2.0-rcsb_download.sdf.
-Parsing SDF file.
-Canonicalizing atom names.
-Assign atom type names.
-Running Epik.
-Epik run completed.
-Assigning charges to protonation states.
-State 1
-Charging completed.
-Writing Epik data for state 1
-Run completed.
-Status: Success</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Verdana"/>
-          </rPr>
-          <t>New run:
-PDB code: SO4; Molecule: Sulfate anion_pH_5.0; pH 5.0
-Retrieving PDB structure from RCSB ligand expo: Sulfate anion_pH_5.0-rcsb_download.pdb.
-Parsing PDB file.
-Retrieving SDF structure from RCSB ligand expo: Sulfate anion_pH_5.0-rcsb_download.sdf.
-Parsing SDF file.
-Canonicalizing atom names.
-Assign atom type names.
-Running Epik.
-Epik run completed.
-Assigning charges to protonation states.
-State 1
-Charging completed.
-Writing Epik data for state 1
-Run completed.
-Status: Success</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E6" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Verdana"/>
-          </rPr>
-          <t>New run:
-PDB code: SO4; Molecule: Sulfate anion_pH_12.0; pH 12.0
-Retrieving PDB structure from RCSB ligand expo: Sulfate anion_pH_12.0-rcsb_download.pdb.
-Parsing PDB file.
-Retrieving SDF structure from RCSB ligand expo: Sulfate anion_pH_12.0-rcsb_download.sdf.
-Parsing SDF file.
-Canonicalizing atom names.
-Assign atom type names.
-Running Epik.
-Epik run completed.
-Assigning charges to protonation states.
-State 1
-Charging completed.
-Writing Epik data for state 1
-Run completed.
-Status: Success</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="105">
   <si>
     <t>Ligand ID</t>
   </si>
@@ -198,9 +42,6 @@
   </si>
   <si>
     <t>PO4</t>
-  </si>
-  <si>
-    <t>See comment for log.</t>
   </si>
   <si>
     <t>ADP</t>
@@ -881,10 +722,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0"/>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
@@ -909,536 +750,466 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2">
+    <row r="2" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
+      <c r="D5" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>18</v>
+        <v>93</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>19</v>
+        <v>94</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>91</v>
+        <v>19</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1448,12 +1219,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0"/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1486,60 +1257,39 @@
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
+      <c r="D2"/>
+      <c r="E2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
+      <c r="D3"/>
+      <c r="E3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D4"/>
+      <c r="E4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
+      <c r="D5"/>
+      <c r="E5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
+      <c r="D6"/>
+      <c r="E6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>